<commit_message>
updated part 2 results
</commit_message>
<xml_diff>
--- a/Part_2_tables/match_on_title_df_grouped.xlsx
+++ b/Part_2_tables/match_on_title_df_grouped.xlsx
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>95</v>
+        <v>9781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>